<commit_message>
implement images in list of posts
</commit_message>
<xml_diff>
--- a/excel/Competencias Finales.xlsx
+++ b/excel/Competencias Finales.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariacachomorgado/Desktop/QUE SERA DE MI/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="987"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="987"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="5" r:id="rId1"/>
@@ -20,9 +15,6 @@
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -2109,7 +2101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2760,7 +2752,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -2795,7 +2787,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -2972,7 +2964,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2982,23 +2974,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.1640625" style="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.5" style="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="106.33203125" style="39" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="39" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.6640625" style="39" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="39"/>
+    <col min="1" max="1" width="22.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.42578125" style="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="106.28515625" style="39" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="39" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="39"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="39" t="s">
         <v>339</v>
       </c>
@@ -3021,7 +3013,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="18.95" customHeight="1">
       <c r="A3" s="39">
         <v>1</v>
       </c>
@@ -3038,7 +3030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="39">
         <v>2</v>
       </c>
@@ -3055,7 +3047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="41">
         <v>3</v>
       </c>
@@ -3069,7 +3061,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="39">
         <v>4</v>
       </c>
@@ -3086,7 +3078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="39">
         <v>5</v>
       </c>
@@ -3109,7 +3101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="39">
         <v>6</v>
       </c>
@@ -3123,7 +3115,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="39">
         <v>7</v>
       </c>
@@ -3137,7 +3129,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="39">
         <v>8</v>
       </c>
@@ -3157,7 +3149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="39">
         <v>9</v>
       </c>
@@ -3174,7 +3166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="39">
         <v>10</v>
       </c>
@@ -3188,7 +3180,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="39">
         <v>11</v>
       </c>
@@ -3208,7 +3200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="42" customFormat="1">
       <c r="A14" s="42">
         <v>12</v>
       </c>
@@ -3222,7 +3214,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="39">
         <v>13</v>
       </c>
@@ -3236,7 +3228,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="42" customFormat="1">
       <c r="A16" s="42">
         <v>14</v>
       </c>
@@ -3257,7 +3249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="39">
         <v>15</v>
       </c>
@@ -3271,7 +3263,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="39">
         <v>16</v>
       </c>
@@ -3288,7 +3280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="39">
         <v>17</v>
       </c>
@@ -3302,7 +3294,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="39">
         <v>18</v>
       </c>
@@ -3317,7 +3309,7 @@
       </c>
       <c r="G20" s="40"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="39">
         <v>19</v>
       </c>
@@ -3331,7 +3323,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="39">
         <v>20</v>
       </c>
@@ -3354,7 +3346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="39">
         <v>21</v>
       </c>
@@ -3371,7 +3363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="39">
         <v>22</v>
       </c>
@@ -3385,7 +3377,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="39">
         <v>23</v>
       </c>
@@ -3415,15 +3407,15 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="43.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.83203125" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="120.6640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="36"/>
+    <col min="1" max="1" width="43.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="120.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="36"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="36" t="s">
         <v>338</v>
       </c>
@@ -3434,7 +3426,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="18.95" customHeight="1">
       <c r="A3" s="36" t="s">
         <v>308</v>
       </c>
@@ -3445,7 +3437,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="36" t="s">
         <v>301</v>
       </c>
@@ -3456,7 +3448,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="37" t="s">
         <v>302</v>
       </c>
@@ -3467,7 +3459,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="36" t="s">
         <v>303</v>
       </c>
@@ -3478,7 +3470,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="36" t="s">
         <v>318</v>
       </c>
@@ -3489,7 +3481,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="21" customHeight="1">
       <c r="A8" s="36" t="s">
         <v>6</v>
       </c>
@@ -3500,7 +3492,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="36" t="s">
         <v>8</v>
       </c>
@@ -3511,7 +3503,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="36" t="s">
         <v>10</v>
       </c>
@@ -3522,7 +3514,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="36" t="s">
         <v>304</v>
       </c>
@@ -3533,7 +3525,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="36" t="s">
         <v>317</v>
       </c>
@@ -3544,7 +3536,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="36" t="s">
         <v>14</v>
       </c>
@@ -3555,7 +3547,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" s="38" customFormat="1">
       <c r="A14" s="38" t="s">
         <v>16</v>
       </c>
@@ -3566,7 +3558,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="36" t="s">
         <v>18</v>
       </c>
@@ -3577,7 +3569,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="38" customFormat="1">
       <c r="A16" s="38" t="s">
         <v>305</v>
       </c>
@@ -3588,7 +3580,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="36" t="s">
         <v>21</v>
       </c>
@@ -3599,7 +3591,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="36" t="s">
         <v>22</v>
       </c>
@@ -3610,7 +3602,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="36" t="s">
         <v>306</v>
       </c>
@@ -3621,7 +3613,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="36" t="s">
         <v>307</v>
       </c>
@@ -3632,7 +3624,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="36" t="s">
         <v>24</v>
       </c>
@@ -3643,7 +3635,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="36" t="s">
         <v>25</v>
       </c>
@@ -3654,7 +3646,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="36" t="s">
         <v>311</v>
       </c>
@@ -3665,7 +3657,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="36" t="s">
         <v>313</v>
       </c>
@@ -3676,7 +3668,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="36" t="s">
         <v>312</v>
       </c>
@@ -3704,9 +3696,9 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -3714,47 +3706,47 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -3776,9 +3768,9 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="B1" t="s">
         <v>41</v>
       </c>
@@ -3795,7 +3787,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3807,7 +3799,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3820,7 +3812,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -3833,7 +3825,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3846,7 +3838,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -3859,7 +3851,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3872,7 +3864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3885,7 +3877,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3898,7 +3890,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3911,7 +3903,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3923,7 +3915,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -3936,7 +3928,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -3948,7 +3940,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -3961,7 +3953,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -3974,7 +3966,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -3986,7 +3978,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3998,7 +3990,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4011,7 +4003,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -4024,7 +4016,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -4037,7 +4029,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -4050,7 +4042,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -4063,7 +4055,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -4076,7 +4068,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4088,7 +4080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4100,13 +4092,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="F27" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -4129,7 +4121,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>1</v>
       </c>
@@ -4149,7 +4141,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="15.75">
       <c r="A31">
         <v>2</v>
       </c>
@@ -4169,7 +4161,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>3</v>
       </c>
@@ -4189,7 +4181,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="15.75">
       <c r="A33">
         <v>4</v>
       </c>
@@ -4209,7 +4201,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>5</v>
       </c>
@@ -4226,7 +4218,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="15.75">
       <c r="A35">
         <v>6</v>
       </c>
@@ -4249,7 +4241,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>7</v>
       </c>
@@ -4269,7 +4261,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9">
       <c r="A37">
         <v>8</v>
       </c>
@@ -4286,7 +4278,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9">
       <c r="A38">
         <v>9</v>
       </c>
@@ -4306,7 +4298,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="15.75">
       <c r="A39">
         <v>10</v>
       </c>
@@ -4326,7 +4318,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="15.75">
       <c r="A40">
         <v>11</v>
       </c>
@@ -4346,7 +4338,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9">
       <c r="A41">
         <v>12</v>
       </c>
@@ -4366,7 +4358,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="15.75">
       <c r="A42">
         <v>13</v>
       </c>
@@ -4390,7 +4382,7 @@
       </c>
       <c r="I42" s="14"/>
     </row>
-    <row r="43" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="15.75">
       <c r="A43">
         <v>14</v>
       </c>
@@ -4413,7 +4405,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="15.75">
       <c r="A44">
         <v>15</v>
       </c>
@@ -4436,7 +4428,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9">
       <c r="A45">
         <v>16</v>
       </c>
@@ -4456,7 +4448,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9">
       <c r="A46">
         <v>17</v>
       </c>
@@ -4473,7 +4465,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="15.75">
       <c r="A47">
         <v>18</v>
       </c>
@@ -4493,7 +4485,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="15.75">
       <c r="A48">
         <v>19</v>
       </c>
@@ -4516,7 +4508,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" ht="15.75">
       <c r="A49">
         <v>20</v>
       </c>
@@ -4539,7 +4531,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8">
       <c r="A50">
         <v>21</v>
       </c>
@@ -4556,7 +4548,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8">
       <c r="A51">
         <v>22</v>
       </c>
@@ -4573,7 +4565,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8">
       <c r="A52">
         <v>23</v>
       </c>
@@ -4590,7 +4582,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8">
       <c r="A53">
         <v>24</v>
       </c>
@@ -4607,7 +4599,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8">
       <c r="A54">
         <v>25</v>
       </c>
@@ -4627,7 +4619,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8">
       <c r="A55">
         <v>26</v>
       </c>
@@ -4644,7 +4636,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8">
       <c r="A56">
         <v>27</v>
       </c>
@@ -4661,16 +4653,16 @@
         <v>132</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8">
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8">
       <c r="B58" t="s">
         <v>43</v>
       </c>
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" ht="15.75">
       <c r="A59">
         <v>1</v>
       </c>
@@ -4687,7 +4679,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8">
       <c r="A60">
         <v>2</v>
       </c>
@@ -4704,7 +4696,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8">
       <c r="A61">
         <v>3</v>
       </c>
@@ -4721,7 +4713,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8">
       <c r="A62">
         <v>4</v>
       </c>
@@ -4739,7 +4731,7 @@
       </c>
       <c r="H62" s="1"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8">
       <c r="A63">
         <v>5</v>
       </c>
@@ -4756,7 +4748,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8">
       <c r="A64">
         <v>6</v>
       </c>
@@ -4773,7 +4765,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" ht="15.75">
       <c r="A65">
         <v>7</v>
       </c>
@@ -4793,7 +4785,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" ht="15.75">
       <c r="A66">
         <v>8</v>
       </c>
@@ -4813,7 +4805,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" ht="15.75">
       <c r="A67">
         <v>9</v>
       </c>
@@ -4833,7 +4825,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" ht="15.75">
       <c r="A68">
         <v>10</v>
       </c>
@@ -4853,7 +4845,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7">
       <c r="A69">
         <v>11</v>
       </c>
@@ -4870,7 +4862,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7">
       <c r="A70">
         <v>12</v>
       </c>
@@ -4887,7 +4879,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7">
       <c r="A71">
         <v>13</v>
       </c>
@@ -4904,7 +4896,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" ht="15.75">
       <c r="A72">
         <v>14</v>
       </c>
@@ -4921,7 +4913,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7">
       <c r="A73">
         <v>15</v>
       </c>
@@ -4938,7 +4930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="15.75">
       <c r="A74">
         <v>16</v>
       </c>
@@ -4958,7 +4950,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7">
       <c r="A75">
         <v>17</v>
       </c>
@@ -4975,7 +4967,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" ht="15.75">
       <c r="A76">
         <v>18</v>
       </c>
@@ -4995,7 +4987,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7">
       <c r="A77">
         <v>19</v>
       </c>
@@ -5012,7 +5004,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7">
       <c r="A78">
         <v>20</v>
       </c>
@@ -5029,7 +5021,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" ht="15.75">
       <c r="A79">
         <v>21</v>
       </c>
@@ -5049,7 +5041,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7">
       <c r="A80">
         <v>22</v>
       </c>
@@ -5066,7 +5058,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7">
       <c r="A81">
         <v>23</v>
       </c>
@@ -5083,7 +5075,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="15.75">
       <c r="A82">
         <v>24</v>
       </c>
@@ -5103,7 +5095,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="15.75">
       <c r="A83">
         <v>25</v>
       </c>
@@ -5123,7 +5115,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7">
       <c r="A84">
         <v>26</v>
       </c>
@@ -5140,7 +5132,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7">
       <c r="A85">
         <v>27</v>
       </c>
@@ -5157,7 +5149,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" ht="15.75">
       <c r="A86">
         <v>28</v>
       </c>
@@ -5177,7 +5169,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7">
       <c r="A87">
         <v>29</v>
       </c>
@@ -5197,7 +5189,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7">
       <c r="A88">
         <v>30</v>
       </c>
@@ -5214,7 +5206,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" ht="15.75">
       <c r="A89">
         <v>31</v>
       </c>
@@ -5234,7 +5226,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" ht="15.75">
       <c r="A90">
         <v>32</v>
       </c>
@@ -5254,7 +5246,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7">
       <c r="A91">
         <v>33</v>
       </c>
@@ -5274,7 +5266,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7">
       <c r="A92">
         <v>34</v>
       </c>
@@ -5291,19 +5283,19 @@
         <v>75</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7">
       <c r="B93" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7">
       <c r="B94" s="26" t="s">
         <v>176</v>
       </c>
       <c r="C94" s="26"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7">
       <c r="A95">
         <v>1</v>
       </c>
@@ -5321,7 +5313,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" ht="15.75">
       <c r="A96">
         <v>2</v>
       </c>
@@ -5342,7 +5334,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7">
       <c r="A97">
         <v>3</v>
       </c>
@@ -5360,7 +5352,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7">
       <c r="A98">
         <v>4</v>
       </c>
@@ -5378,7 +5370,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7">
       <c r="A99">
         <v>5</v>
       </c>
@@ -5396,7 +5388,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7">
       <c r="A100">
         <v>6</v>
       </c>
@@ -5414,7 +5406,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7">
       <c r="A101">
         <v>7</v>
       </c>
@@ -5432,7 +5424,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" ht="15.75">
       <c r="A102">
         <v>8</v>
       </c>
@@ -5453,13 +5445,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7">
       <c r="B103" s="26" t="s">
         <v>180</v>
       </c>
       <c r="C103" s="26"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7">
       <c r="A104">
         <v>9</v>
       </c>
@@ -5477,7 +5469,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7">
       <c r="A105">
         <v>10</v>
       </c>
@@ -5495,7 +5487,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7">
       <c r="A106">
         <v>11</v>
       </c>
@@ -5513,7 +5505,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" ht="15.75">
       <c r="A107">
         <v>12</v>
       </c>
@@ -5534,7 +5526,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7">
       <c r="A108">
         <v>13</v>
       </c>
@@ -5552,7 +5544,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" ht="15.75">
       <c r="A109">
         <v>14</v>
       </c>
@@ -5573,7 +5565,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7">
       <c r="A110">
         <v>15</v>
       </c>
@@ -5591,13 +5583,13 @@
         <v>125</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7">
       <c r="B111" s="26" t="s">
         <v>187</v>
       </c>
       <c r="C111" s="26"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7">
       <c r="A112">
         <v>16</v>
       </c>
@@ -5615,7 +5607,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" ht="15.75">
       <c r="A113">
         <v>17</v>
       </c>
@@ -5633,7 +5625,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" ht="15.75">
       <c r="A114">
         <v>18</v>
       </c>
@@ -5654,7 +5646,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" ht="15.75">
       <c r="A115">
         <v>19</v>
       </c>
@@ -5675,7 +5667,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7">
       <c r="A116">
         <v>20</v>
       </c>
@@ -5693,7 +5685,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" ht="15.75">
       <c r="A117">
         <v>21</v>
       </c>
@@ -5714,7 +5706,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7">
       <c r="A118">
         <v>22</v>
       </c>
@@ -5732,7 +5724,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7">
       <c r="A119">
         <v>23</v>
       </c>
@@ -5750,13 +5742,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7">
       <c r="B120" s="26" t="s">
         <v>194</v>
       </c>
       <c r="C120" s="26"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7">
       <c r="A121">
         <v>24</v>
       </c>
@@ -5774,7 +5766,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7">
       <c r="A122">
         <v>25</v>
       </c>
@@ -5792,7 +5784,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7">
       <c r="A123">
         <v>26</v>
       </c>
@@ -5810,7 +5802,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" ht="15.75">
       <c r="A124">
         <v>27</v>
       </c>
@@ -5828,7 +5820,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" ht="15.75">
       <c r="A125">
         <v>28</v>
       </c>
@@ -5849,7 +5841,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7">
       <c r="A126">
         <v>29</v>
       </c>
@@ -5867,7 +5859,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" ht="15.75">
       <c r="A127">
         <v>30</v>
       </c>
@@ -5888,7 +5880,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7">
       <c r="A128">
         <v>31</v>
       </c>
@@ -5906,7 +5898,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7">
       <c r="A129">
         <v>32</v>
       </c>
@@ -5947,294 +5939,294 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="90" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="90">
       <c r="A2" s="29" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="150" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" ht="165">
       <c r="A3" s="29" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" ht="60">
       <c r="A4" s="29" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="90" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" ht="105">
       <c r="A5" s="29" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="90" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" ht="120">
       <c r="A6" s="29" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="90" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" ht="90">
       <c r="A7" s="29" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" ht="75">
       <c r="A8" s="29" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1">
       <c r="A11" s="30" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1">
       <c r="A12" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1">
       <c r="A15" s="30" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" s="31" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" s="31" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1">
       <c r="A21" s="30" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1">
       <c r="A22" s="30" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1">
       <c r="A23" s="30" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1">
       <c r="A24" s="30" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1">
       <c r="A25" s="30" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1">
       <c r="A26" s="30" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1">
       <c r="A27" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" ht="90">
       <c r="A28" s="29" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1">
       <c r="A29" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1">
       <c r="A30" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1">
       <c r="A31" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1">
       <c r="A32" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" ht="15.75">
       <c r="A33" s="8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" ht="15.75">
       <c r="A35" s="8" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1">
       <c r="A36" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" ht="15.75">
       <c r="A37" s="8" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1">
       <c r="A38" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" ht="15.75">
       <c r="A39" s="8" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1">
       <c r="A40" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1">
       <c r="A41" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" ht="15.75">
       <c r="A42" s="8" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1">
       <c r="A43" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1">
       <c r="A44" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" ht="15.75">
       <c r="A45" s="8" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1">
       <c r="A46" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" ht="15.75">
       <c r="A47" s="8" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1">
       <c r="A48" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" ht="15.75">
       <c r="A50" s="8" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" ht="15.75">
       <c r="A53" s="8" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" ht="15.75">
       <c r="A54" s="8" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" ht="15.75">
       <c r="A57" s="8" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" ht="15.75">
       <c r="A61" s="32" t="s">
         <v>133</v>
       </c>
@@ -6242,7 +6234,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2">
       <c r="A62" s="34" t="s">
         <v>82</v>
       </c>
@@ -6250,7 +6242,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" ht="60">
       <c r="A63" s="35" t="s">
         <v>264</v>
       </c>
@@ -6258,7 +6250,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2">
       <c r="A64" s="34" t="s">
         <v>136</v>
       </c>
@@ -6266,7 +6258,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2">
       <c r="A65" s="34" t="s">
         <v>104</v>
       </c>
@@ -6274,7 +6266,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2">
       <c r="A66" s="34" t="s">
         <v>86</v>
       </c>
@@ -6282,10 +6274,10 @@
         <v>268</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" ht="15.75">
       <c r="A68" s="32" t="s">
         <v>138</v>
       </c>
@@ -6293,7 +6285,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2">
       <c r="A69" s="34" t="s">
         <v>141</v>
       </c>
@@ -6301,7 +6293,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2">
       <c r="A70" s="34" t="s">
         <v>111</v>
       </c>
@@ -6309,7 +6301,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2">
       <c r="A71" s="34" t="s">
         <v>74</v>
       </c>
@@ -6317,7 +6309,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2">
       <c r="A72" s="34" t="s">
         <v>145</v>
       </c>
@@ -6325,7 +6317,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2">
       <c r="A73" s="34" t="s">
         <v>148</v>
       </c>
@@ -6333,7 +6325,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2">
       <c r="A74" s="34" t="s">
         <v>151</v>
       </c>
@@ -6341,10 +6333,10 @@
         <v>275</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2">
       <c r="A75" s="1"/>
     </row>
-    <row r="76" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" ht="15.75">
       <c r="A76" s="32" t="s">
         <v>89</v>
       </c>
@@ -6352,7 +6344,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2">
       <c r="A77" s="34" t="s">
         <v>152</v>
       </c>
@@ -6360,7 +6352,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2">
       <c r="A78" s="34" t="s">
         <v>154</v>
       </c>
@@ -6368,7 +6360,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2">
       <c r="A79" s="34" t="s">
         <v>95</v>
       </c>
@@ -6376,7 +6368,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2">
       <c r="A80" s="34" t="s">
         <v>157</v>
       </c>
@@ -6384,7 +6376,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2">
       <c r="A81" s="34" t="s">
         <v>160</v>
       </c>
@@ -6392,7 +6384,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2">
       <c r="A82" s="34" t="s">
         <v>108</v>
       </c>
@@ -6400,7 +6392,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2">
       <c r="A83" s="34" t="s">
         <v>67</v>
       </c>
@@ -6408,7 +6400,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2">
       <c r="A84" s="34" t="s">
         <v>161</v>
       </c>
@@ -6416,7 +6408,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2">
       <c r="A85" s="34" t="s">
         <v>162</v>
       </c>
@@ -6424,7 +6416,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2">
       <c r="A86" s="34" t="s">
         <v>114</v>
       </c>
@@ -6432,7 +6424,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2">
       <c r="A87" s="34" t="s">
         <v>101</v>
       </c>
@@ -6440,7 +6432,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2">
       <c r="A88" s="34" t="s">
         <v>123</v>
       </c>
@@ -6448,7 +6440,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2">
       <c r="A89" s="34" t="s">
         <v>166</v>
       </c>
@@ -6456,7 +6448,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2">
       <c r="A90" s="34" t="s">
         <v>92</v>
       </c>
@@ -6464,7 +6456,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2">
       <c r="A91" s="34" t="s">
         <v>168</v>
       </c>
@@ -6472,7 +6464,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2">
       <c r="A92" s="34" t="s">
         <v>70</v>
       </c>
@@ -6480,7 +6472,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2">
       <c r="A93" s="34" t="s">
         <v>170</v>
       </c>
@@ -6488,7 +6480,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2">
       <c r="A94" s="34" t="s">
         <v>172</v>
       </c>
@@ -6496,7 +6488,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2">
       <c r="A95" s="34" t="s">
         <v>174</v>
       </c>
@@ -6504,7 +6496,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2">
       <c r="A96" s="34" t="s">
         <v>75</v>
       </c>
@@ -6512,207 +6504,207 @@
         <v>296</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1">
       <c r="A98" s="1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1">
       <c r="A99" s="26" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1">
       <c r="A100" s="26" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1">
       <c r="A101" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1">
       <c r="A102" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1">
       <c r="A103" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1">
       <c r="A104" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1">
       <c r="A105" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1">
       <c r="A106" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1">
       <c r="A107" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1">
       <c r="A108" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1">
       <c r="A109" s="26" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1">
       <c r="A110" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1">
       <c r="A111" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1">
       <c r="A112" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1">
       <c r="A113" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1">
       <c r="A114" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1">
       <c r="A115" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1">
       <c r="A116" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1">
       <c r="A117" s="26" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1">
       <c r="A118" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1">
       <c r="A119" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1">
       <c r="A120" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1">
       <c r="A121" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1">
       <c r="A122" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1">
       <c r="A123" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1">
       <c r="A124" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1">
       <c r="A125" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1">
       <c r="A126" s="26" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1">
       <c r="A127" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1">
       <c r="A128" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1">
       <c r="A129" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1">
       <c r="A130" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1">
       <c r="A131" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1">
       <c r="A132" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1">
       <c r="A133" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1">
       <c r="A134" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1">
       <c r="A135" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1">
       <c r="A137" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1">
       <c r="A138" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1">
       <c r="A139" t="s">
         <v>65</v>
       </c>

</xml_diff>